<commit_message>
Get daily reddit data: Tue Apr 22 08:12:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_27.xlsx
+++ b/data/collected_data/2025_04_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C474"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2947 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1k501nv</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>My failed attempt at soap nails :/</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5g89pjcs3cwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1k4za58</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Simple sparkles for Easter. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4za58</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1k4z7fz</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Did I go too far 😂</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4z7fz</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1k4z781</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Spring nails!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4z781</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1k4z36u</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Subtle Colour Nails</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azarekl3sbwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1k4yslj</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>💜🦄</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oq7dxf9mobwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1k4ymm5</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>What are these lines on my nails and what can i do about them?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42u57ukqmbwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1k4ym7w</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Late Easter Nails!</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4ym7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1k4y99h</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>where to buy magnetic heart tool</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4y99h/where_to_buy_magnetic_heart_tool/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1k4y3wc</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Do I need a separate primer?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c56ipc0ygbwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1k4wyux</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Help me troubleshoot my press-ons!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4wyux/help_me_troubleshoot_my_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1k4w3tw</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Some fav sets I did recently</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4w3tw</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1k4x66n</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Floral nails</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4x66n</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1k4xnv9</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Mirror Gel Turning Gray??</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4xnv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1k4x80n</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>My koi fish nails ✨️</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2xzhrep7bwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1k4wdjd</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Gel polish brand</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4wdjd/gel_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1k4wc9r</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Decided to do some simple flowers today 🦋🩵💙</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsq2i4l8zawe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1k4w08m</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Why does gel polish peel off in sheets on my natural nails?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4w08m/why_does_gel_polish_peel_off_in_sheets_on_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1k4vtda</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Are nail techs supposed to do and detailed filing before putting on a new set?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4vtda/are_nail_techs_supposed_to_do_and_detailed_filing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1k4p23i</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>starting my journey to do nails professionally, any tips?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4p23i/starting_my_journey_to_do_nails_professionally/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1k4vvo8</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Did these eat?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cxg1wbvuawe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1k4pp20</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Fluttering into the week with these butterfly beauties 🦋💖</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71ppnd36e9we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1k4s206</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>My pinky nail just tore right up when I jammed it into the door knob. Earlier this week something similar but not nearly as bad happened to another finger. I just got my acrylics done 9 days ago.</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/085j6lflw9we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1k4p2am</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Cuticle remover (I f*** up)</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4p2am/cuticle_remover_i_f_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1k4qucs</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>At what point do you ask for a fill vs new set?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3q0dqd3n9we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1k4s742</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Mini-egg inspired gel press-ons! (Inspo from u/zefeara)</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4s742</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1k4ti3a</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>ruined nails..</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff4z8pxe9awe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1k4uzl2</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Cherry nail art.</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hssmgwrmawe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1k4uyfd</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Diseño ojo de gato</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46if3sygmawe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1k4ujps</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Keep calm and let your nails do the talking.</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybz5gmdkiawe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1k4ub9i</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Another cute set for the week! I missed putting charms and decorations in them.</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4ub9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1k4uavv</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Que tal quedaron ?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fwaonkggawe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1k4ua1k</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Hermosas?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b86qh0c8gawe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1k4u32z</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>BIAB?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4u32z/biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1k4txaj</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3my5gi3dawe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1k4thsa</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Press on nail business</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4thsa/press_on_nail_business/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1k4t8qm</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>i’m starting my own business selling fake nails and i’m wanting to include little primers with them, but the containers i bought, the primer ate right through them :( do i need glass bottles? would it eat through stoppers too?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4t8qm/im_starting_my_own_business_selling_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1k4rt8z</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>color block twist on a french mani 💙</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4rt8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1k4rk7l</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Press ons!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4rk7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1k4rd1u</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>In love with cat eye</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4rd1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1k4qmef</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Starting to get my nails done again</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxf8opebl9we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1k4qjov</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>When the nails match the book🩵☁️</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpbkqaupk9we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1k4pzzr</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Manifesting summer</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pv8c72ig9we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1k4pv1j</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>2 nails of my expensive manicure from 2.5 weeks ago have come off.. are salons expected to fix them for free or I have to wait it out till my next refill?😭😭</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4pv1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1k4p7qf</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>😍</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5crt7r9ka9we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1k4ovur</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>First time they made actually them short when I asked</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azshlzj489we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1k4ovol</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Safest gel nail polish</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4ovol/safest_gel_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1k4ojdt</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>First ever press-ons haul</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4ojdt</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1k4o511</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Floral nail art 💅</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4o511</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1k4nzh7</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>What nail glue and glue remover can I use to reuse press-on nails without damaging my natural nails?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4nzh7/what_nail_glue_and_glue_remover_can_i_use_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1k4o1ah</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>my 2nd gel-x attempt</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bechujzt19we1</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1k4nzeb</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>My current spring manicure</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4nzeb</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1k4c67a</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>What is up with my nails???</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4c67a</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1k4nh1h</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Need advise and have some questions</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4nh1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1k4nm1t</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>is this normal?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sug055ty8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1k4nbzo</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Gel x none of it works</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4nbzo/gel_x_none_of_it_works/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1k4n23m</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Took my gel off</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4n23m</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1k4mk6d</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>How do I improve my cuticle?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4mk6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1k4klyo</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Nails and more nails.</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4klyo/nails_and_more_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1k4b1o5</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>How do I fix downward-curved nails?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4b1o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1k4lsnz</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>got my nails done and now my nail bed is shrinking?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4lsnz/got_my_nails_done_and_now_my_nail_bed_is_shrinking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1k4mzfg</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Opinions on my natural nails</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gvoc8t59u8we1</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1k4min3</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Yet another killer set 💜💅🏻</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6frf30mvq8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1k4m67z</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>RAWR. XD</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2k6miwqdo8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1k4m4rl</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Very Cruella Deville Vibes</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylshrr24o8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1k4lquj</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Starry sky nails 🌌</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4lquj</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1k4lorm</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>First time doing my nails by myself</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4lorm</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1k4lko9</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>simple but cute</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tan69695k8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1k4lgt9</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>new nails &lt;33</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4lgt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1k4l192</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Round 4 of doing my own builder and I think I’m getting there.</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4l192</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1k4kvqf</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>New set (thank goodness)</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m46gs5y8f8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1k4kfbi</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>First time Russian manicure</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4kfbi/first_time_russian_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1k4k4st</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Milky White for the Win!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lh36f00a8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1k4jz7b</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Little sister popped off 💅👑</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4jz7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1k4barc</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Why do my nails get little breaks on the sides to the point where they end up breaking and I have to cut them? How can I prevent this/manage this?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4barc/why_do_my_nails_get_little_breaks_on_the_sides_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1k4eaff</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Geo tip question</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4eaff/geo_tip_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1k4jj0b</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Press on win!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4jj0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1k4jhpb</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>A day late but happy 4/20!</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4jhpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1k4ing3</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Blueberry and lime</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4ing3</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1k4ilf7</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jonw4u8dz7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1k4i4k4</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Me and My sisters easter nails (as a beginner)</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0tbzhf6w7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1k4i3tp</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Gel pedicure polish only?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4i3tp/gel_pedicure_polish_only/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1k4i10q</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4i10q</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1k4i0ac</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>♡</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oa838ilcv7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1k4hxyz</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>I love my little snake friend!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4hxyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1k4hrvq</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Spiced up basic nails with a bit of subtle art</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4hrvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1k4h8g9</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Help!! Broken nail?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tda60l9xp7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1k4gso3</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Just took a tumble</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1aj4cpmrm7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1k4gr6x</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>My first nails as a beginner!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4gr6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1k4gm03</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Spring green, anyone? 💚🌿</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4gm03</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1k4f3lw</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Best diy at home manicure for beginners?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4f3lw/best_diy_at_home_manicure_for_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1k4ghup</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>It is the first time I do sculptured nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwgmadn6j7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1k4gcd6</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>My nail tech also gave me the best pedi ever 🥹</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4ytjah4i7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1k4e9hq</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>First time using builder gel!</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fomgfhzp27we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1k4fw4g</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>bday nails for my client 🌊🐠</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vm7rogove7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1k4fvpc</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Chameleon Cutie</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4fvpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1k4fkes</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Contact Dermatitis</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k4fkes/contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1k4fmrk</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Sensory nightmare</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4fmrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1k4fhyp</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Neutral Nails</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpzh0gg2c7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1k4f9aa</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>My nail tech is a perfectionist</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x50c3ro9a7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1k4zso6</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>All That by LynBDesigns</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4zso6</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1k4y9bh</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>CND Super Shiny Top Coat Replacement?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k4y9bh/cnd_super_shiny_top_coat_replacement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1k4xpo9</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Magical cats</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4xpo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1k4wvtr</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Cracked Polish Skittle</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4wvtr</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1k4wuv1</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>I had a vision for a lavender spring set, and I LOVE how it came out!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd88ud544bwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1k4w22l</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Mournicure for a Dope Pope</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27jg2qckwawe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1k4w1l8</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>wow 🤩</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4w1l8</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1k4vuuh</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>which of the forces to choose?</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4vuuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1k4vft9</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Cirque Refer a Friend?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4vft9</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1k4utcj</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Dead Nettle</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuijk006lawe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1k4uifq</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Last day for these Easter nails</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4u3za8fiawe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1k4uhqd</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>ILNP Willow- didn’t expect to like it, but I do</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vancp7g8iawe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1k4tpnl</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Nail Shaping</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k4tpnl/nail_shaping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1k4thp0</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Lurid My Five Hundred Year Old Boyfriend</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k4thp0/lurid_my_five_hundred_year_old_boyfriend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1k4t73l</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>How is this magnetic effect achieved?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fos763p6awe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1k4t363</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>🎵there's a flicker of light...</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k006htzn5awe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1k4skwp</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Once in a blue moon, I find the motivation to do nail art. This weekend was one such occasion.</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4skwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1k4s04d</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Aurora plastic film</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgu8ov8iw9we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1k4rrfj</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>A sparkly palate cleanser!</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nonyh5kcu9we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1k4rdxt</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Napa mani recommendations?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k4rdxt/napa_mani_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1k4r3v3</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Layered something impossibly sparkly over something impossibly shifty</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4r3v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1k4qth5</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Does anyone know what this is? The store told me it was nail oil, but it smells like acetone and becomes tacky immediately after being applied to the skin - gonna guess it’s not nail oil</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4qth5</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1k4q5ed</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Accidentally matching a little too well</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84ed5vjoh9we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1k4phq9</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>big chop + trying a new shape</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4phq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1k4ex4x</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Sakura love</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4ex4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1k4ikgl</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Canadian company’s</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k4ikgl/canadian_companys/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1k4op6z</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>My version of "clean girl" nails</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4op6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1k4lh0r</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Question about my nails</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4lh0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1k4omil</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>3D art: annoying or no?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4n6s27s669we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1k4nsyv</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Revlon Vixen is the perfect vampy red 🍷</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4nsyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1k4ngnv</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Mooncat Earth to Gaia vs Cirque Paradiso?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4ngnv</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1k4mx7i</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>✨Fancy Fingers✨ GUCCI</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzhhayftt8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1k4mrz0</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Dove Jelly</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4mrz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1k4miq2</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Are some of you sleeping on Lurid Lacquer??</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k4miq2/are_some_of_you_sleeping_on_lurid_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1k4lvyp</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>first nail casualty in my new jeep 😒</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4lvyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1k4lr8z</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Where can I find a color like this Starbucks cup?</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr2cmq1fl8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1k4lcol</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Bought Canadian 🇨🇦</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39or3t5li8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1k4l8i3</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>La Colors FTW</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4l8i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1k4ku8t</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>blue skittle for Monday 💙</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4ku8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1k4kbd8</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Like candy eggs 🪺</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4kbd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1k4k6ti</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>some new Doom Loop Corrupted shades 🌈</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4k6ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1k4k1sx</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Is this possible with regular polish?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4k1sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1k4jyvo</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>FEELS SO GOOD TO HAVE MY NAILS DONE AGAIN 😭</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0a6127mw88we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1k4jdjr</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Easter Mani</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg59836u48we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1k4j1p6</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Extremely brittle toenails. Please help!</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k4j1p6/extremely_brittle_toenails_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1k4iqir</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Copyright Policy notice.  Anyone else?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k4iqir/copyright_policy_notice_anyone_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1k4i21e</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Gradient to start off the week!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pmvpt6pv7we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1k4foh8</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Chunky glitter gradient ✨</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0belhaw8d7we1</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1k4fj09</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Easter nail art inspired by traditional Czech egg painting, officially called "kraslice" 🥚🇨🇿</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4fj09</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1k4fco2</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>🌟🌌Starry Night🌌🌜</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4fco2</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1k4ea9j</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>A pink starry moment</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4ea9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1k4dv79</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Love this community</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4dv79</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1k4bsig</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Painting minis and I keep being distracted by my nails</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bxl0bazch6we1</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1k4bnuv</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Traffic cone inspired</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4bnuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1k4ba5t</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>I tried the new P-Gel</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1l8acau8c6we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1k4b4em</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>does this work with my skintone?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg8qxglka6we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1k49uy8</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k49uy8/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1k50xbn</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Ocean set 🌊🐙🦈💙💙💙</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k50xbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1k50wax</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Ocean set 🐙🦈🌊💙💙💙</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v09cgv6wecwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1k50rxc</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Bioluminescence jellyfish 🪼</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k50rxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1k50r9u</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Loving these hehe</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k50r9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1k4xp54</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Starting my nail art journey</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vx8lg79hcbwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1k4wwrf</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Current Spring Manicure</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4wwrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1k4v1kt</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>My Cherry nails 🍒</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5qcwip8nawe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1k4q9z6</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Scooby nails 🙈</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4q9z6</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1k4ph3q</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>✨️💛</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihq70buhc9we1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1k4p0tc</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Some Nail Art I've done</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4p0tc</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1k4oc5q</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Show off</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4oc5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1k4o89x</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>My first nail art a while ago</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l74wssia39we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1k4o3gh</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>First post in group hiii here's my attempt at aura nails</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4o3gh</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1k4mko9</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>new set for the week</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g81lvjbar8we1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1k4gu6n</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>My first nails as a beginner</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k4gu6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1k4f43q</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>New tutorial just dropped for this set!</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnto057697we1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Apr 23 08:12:28 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_27.xlsx
+++ b/data/collected_data/2025_04_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C474"/>
+  <dimension ref="A1:C664"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8491,6 +8491,3236 @@
         </is>
       </c>
     </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1k5t730</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Florals for spring. Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5t730</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1k5t1gs</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Assistance with my first efile please?:)</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncwf3ny8bjwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1k5rqtl</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Learning how to do my own nails and need advice</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5rqtl</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1k5mxdg</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>What do I do now?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5mxdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1k5qtw1</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>tacky and gaudy; on me by me :)</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0348kinzkiwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1k5rb5j</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Sanrio my go to🩷🤍</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxiek96cqiwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1k5r7xf</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>do these remind you of chiclets</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5r7xf</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1k5qqwt</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>obsessed with how my opalscent nails look in the sun ☻️</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dff8lj64kiwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1k5p7tr</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>I don't know if this is normal—should I go back to the salon?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5p7tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1k5ny71</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Green nail after acrylic popped off</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ccw9m2qshwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1k5oxod</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>$150 nails breaking 2 days after getting them done 🥲</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5oxod</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1k5pwf6</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Nails of the week!!</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5pwf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1k5pq2y</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Saying goodbye :(</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hc4fatof9iwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1k5pbwl</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>How many coats of polish do you normally do?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5pbwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1k5pagg</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Nude Cat Eye</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5pagg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1k5oj8e</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>not sure how i feel about thesee 🙃</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ua35ue80yhwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1k5of0k</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Cutie nails for my client!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yud8vl7ywhwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1k5oakb</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Do these eat?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6uu9zbvvhwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1k5o9nx</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Gel alternative</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5o9nx/gel_alternative/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1k5o4p1</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Wedding Nails 💅</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqxn6m0fuhwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1k5nzwt</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>What do you use to make your press ons stay on the stand?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5nzwt/what_do_you_use_to_make_your_press_ons_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1k5nxsa</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>brat nails for Charli xcx!</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5nxsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1k5n5sj</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Magnetic Polish</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jlne3h0jlhwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1k5n4v0</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Can I use dip base coat as press on glue?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5n4v0/can_i_use_dip_base_coat_as_press_on_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1k5mvv7</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Holographic chrome nails🎀🍇</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5mvv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1k5lln9</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>What is this and does it work?</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jj51nycg7hwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1k5mb9c</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Greek Orthodox Easter nails! 🇬🇷☦️</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5mb9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1k5mnya</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Kitty paws!</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5mnya</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1k5mlj4</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Any tips to DIY these?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3408bpidghwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1k5mkw0</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>New to doing my own nails</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5mkw0/new_to_doing_my_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1k5mkkc</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Tried something new!</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfa5zt65ghwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1k5m9uh</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Experimenting with OPI colors</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwmv9ehidhwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1k5lywd</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>my new press-on nails 🌊🐠🪸</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5lywd</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1k5lwdj</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>This took me hours 😭 please be nice</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5lwdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1k5kl5y</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>😍🥰❤️</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dku59xvygwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1k5ka6l</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Bridal Style 😮</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5ka6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1k5jz33</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Wisteria Themed Nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5jz33</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1k5j54y</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Nails that you don’t need to soak off and can keep getting filled?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5j54y/nails_that_you_dont_need_to_soak_off_and_can_keep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1k5jnw5</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>How do you remove your Kiss imPRESS nails?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5jnw5/how_do_you_remove_your_kiss_impress_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1k5j8yi</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>this but in a Essie or OPI color?!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mad3fss0ogwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1k5j6cl</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>My little pony nails</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb1qwjsfngwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1k5ikng</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Commencer à faire mes ongles moi-même ?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5ikng/commencer_à_faire_mes_ongles_moimême/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1k5hgnn</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Help: Recommendation for father of 3</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5hgnn/help_recommendation_for_father_of_3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1k5i600</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Was using my cat as a background for my nails and she was not impressed.. anyways, they’re cute 🤷🏻‍♀️🤣</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5i600</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1k5hr71</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Simple Spring Set</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8oxmnn6pcgwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1k5hoa1</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Horizontal Dent on Press Ons</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srock3s3cgwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1k5hk1d</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Enchanted nails</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gu8wzko8bgwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1k5hfhw</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Mother Daughter Nail Day</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwhaxrhbagwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1k5h51b</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>This set really doesn't feel like "me"</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5ct56r68gwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1k5gs97</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Opal Galaxies🌌✨</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/viqsxcle5gwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1k5gk1g</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Spring gel floral</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5gk1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1k5g1xo</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Acrylic or BIAB extensions for a beach + hike vacation?</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5g1xo/acrylic_or_biab_extensions_for_a_beach_hike/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1k5gb0n</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Butterfly set</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5gb0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1k5gdib</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Do you like them?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5gdib</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1k5g3ub</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Hey I wonder if anyone can tell me what's on trend this summer in the U.S. / UK looking for somethin feminine / spring that I can adapt for short nails and show them (we speak different languages)</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5g3ub/hey_i_wonder_if_anyone_can_tell_me_whats_on_trend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1k5fnhu</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>EPhD nail treatment</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5fnhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1k5fkm8</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>short clean nails</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y44y5hluwfwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1k5fgoh</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5fgoh/male/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1k5fbnh</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>YAYYYYY</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5fbnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1k5f80z</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>btart box X-Coat Tips</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5f80z/btart_box_xcoat_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1k5e677</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Cherry glaze color?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5e677</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1k5ekgh</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>permanently cracked nail after break</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5ekgh/permanently_cracked_nail_after_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1k5f1cu</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Flower vibes.</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5f1cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1k5exyr</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Spring nails 💐</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvcteg1bsfwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1k5eqpq</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Practice For The Day 🦋</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5eqpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1k5dlnh</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Late post - Easter nails</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xj5yvzjvifwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1k5dgdv</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>(Early) Birthday nails! 🎉</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5dgdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1k5cvq5</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>mymelodysusie drill</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3x8z8psdfwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1k5d8f2</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Nail Salons trying to get people to spend more?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9jww3i9gfwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1k5cu3i</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Do you think a nail technician can work on this broken nail?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wir3dghdfwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1k5c8ye</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Broken nail attached to hyponychium</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5c8ye</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1k5cd0x</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>How do you share nail design ideas with your nail artist?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oivxr4p3afwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1k5bhq6</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Is there anything I can do to be able to wear press ons on this nail?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nade10nx3fwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1k5bvv0</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Don’t they look cute!!</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5bvv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1k5bq9p</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Subtle spring flower detail 🌷</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8kzkt5n5fwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1k5bbab</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Self-done experiment</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcekqyrn2fwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1k5bcoa</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Apres VS PLA gel</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5bcoa/apres_vs_pla_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1k5aw8t</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Nails keep lifting at cuticle edge</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5aw8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1k59cg1</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Nail bed side detaching?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnnzua6koewe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1k56nek</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>What happened to my nail??</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewpuvhsg4ewe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1k542fu</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Need help</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k542fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1k50g25</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Nail keeps splitting in the same spot</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k50g25</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1k5aueh</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Perfect theme for Easter lol</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4aj0ms9zewe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1k53z44</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>In LOVE with my little cherry blossoms</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k53z44</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1k5aqtt</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>First time trying new techniques</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9o1e86jyewe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1k5aq49</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>My nail tech is a perfectionist I’m so happy with how they turned out 🌸</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvtf0qaeyewe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1k5amjs</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>The lipstick nails cannot be stopped.</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5amjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1k5ad3z</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>4 best friends 100% ATE at their prom</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5ad3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1k59woq</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>My homemade nails</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k59woq</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1k59vrt</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Delicate yet dark. Love it</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k59vrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1k59af4</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Opinion- how much would you pay for these  :)? (Gelx) Criticism welcome. Anything I can work on ? Thank you 🫶</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k59af4</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1k56dgy</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>My nails keep breaking.  I'm thinking about trying false nails.  Any advice?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k56dgy/my_nails_keep_breaking_im_thinking_about_trying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1k5902q</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Help me decide: Ring Ceremony Nails</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k5902q/help_me_decide_ring_ceremony_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1k58ycr</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>💕 My tech killed this...💕 UT, USA</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k58ycr</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1k58xj7</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Out of this world 🌎 👽🪐🛸✨</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k58xj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1k55nrv</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>I got press ons for the first time!!</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/658253edwdwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1k55eyp</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Cat likes my nails</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k55eyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1k530yz</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Can I fix this?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/541d8lg96dwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1k54cky</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Did my nails! Basic but I love them.</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k54cky/did_my_nails_basic_but_i_love_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1k53h91</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Nail Art for the Cherry blossom festival 🌸</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k53h91</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1k5teju</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Swatching complete (sort of!)</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5teju</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1k5t8sq</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Badly peeling nails</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5t8sq</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1k5t1mf</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>first time doing gel x</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5t1mf</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1k5sqbr</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>BKL Found Family</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5sqbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1k5scmh</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Pinky purple skittle</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5scmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1k5qfzz</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>It's like five colors in one!</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0yl11lwsgiwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1k5qfj3</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Just did my first magnetic velvetized polish!</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qas4j3ungiwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1k5qeol</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | MILF – Multichrome in Lacquer Form</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5qeol</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1k5q8s9</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>🦋 Magnetic Butterflies 🦋</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5q8s9</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1k5onk0</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>I’m in BKLooooooove</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7hupqdy5zhwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1k5mwej</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>LBOH</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5mwej/lboh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1k5mub5</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>River Styx 💚💙</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5mub5</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1k5l6gv</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>How do YOU do cuticle prep?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5l6gv/how_do_you_do_cuticle_prep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1k5kqs0</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Anyone else love a pastel rainbow gradients?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8x942z60hwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1k5kmvj</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Purple glowy shimmer skittle</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5kmvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1k5d760</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>You already know...</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5d760</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1k5k50j</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Accidentally bought doubles😭</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5k50j/accidentally_bought_doubles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1k5jybw</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>What can I use to scent QDTC?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5jybw/what_can_i_use_to_scent_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1k5ja4y</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Over filled my nails 😩</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5ja4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1k5j64e</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>A Little Ranunculus</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5j64e</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1k5j11x</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Mama's nails!</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5j11x</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1k5ip5z</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Eternal Glow💜💖🧡</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5ip5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1k5ij8n</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Smoky / Dusty Blues</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5ij8n/smoky_dusty_blues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1k5idyj</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>So glowy!!</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5idyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1k5i2d0</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>why does a broken nail feel so shameful 🫣</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8fj8zd0fgwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1k5i0la</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Dupe for Cirque Colors Black Magic?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u82fs6cnegwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1k5hguj</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Rocco's Modern Life!</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5hguj</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1k5hd4q</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Phoenix Reborn is simply the bee's knees!</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3t0rnh2t9gwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1k5hbyx</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Spring Time Skittle 🌸🍀🪺</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5hbyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1k5gx5o</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Mama told me not to, I did it anyway - Misbehaving 🎶</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyvndh0m6gwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1k5gw55</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Fav of all time 💚</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6iqbjce6gwe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1k5gl6w</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Boa Constrictor for Earth Day 🪱</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/als7vx264gwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1k5gkr7</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Orly BIAB - Can't make it a day w/o peeling - Help!</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5gkr7/orly_biab_cant_make_it_a_day_wo_peeling_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1k5ggpx</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Worse nails after starting cuticle oil routine? Advice needed</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5ggpx/worse_nails_after_starting_cuticle_oil_routine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1k5gfwf</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Help me decide what polish to wear for an interview?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5gfwf/help_me_decide_what_polish_to_wear_for_an/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1k5g6ud</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Teddy - ILNP</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pary5yen0gwe1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1k5fcn0</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>painted my nails for NHL playoffs! hoping it will be a good luck charm this year 😋</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5fcn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1k5fant</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Fresh nails for my holiday tomorrow!</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5fant</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1k5f3t6</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Do you ever stare at your mani so much you want to paint your nails again?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5f3t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1k5exk2</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>What field of work are you in, and does it affect how you do your nails?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5exk2/what_field_of_work_are_you_in_and_does_it_affect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1k5edps</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>ILNP Petals over Mooncat Jewel Beetle</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dh028p5cofwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1k5e67y</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>🪩🪩Shiny Disco Balls!🪩🪩</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5e67y</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1k5e4dh</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>la la la lava ch ch ch chicken ⛏️</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5e4dh</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1k5e0fa</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Vintage cult classic alongside modern cult classic: blue addition</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5e0fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1k5dr95</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>do you ever just…</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5dr95</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1k5dbyi</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Looking for a pink - peach - orange- yellow shift or magnetic!</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5dbyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1k5coo5</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Found my Favorite Stamping Combo</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5coo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1k5c73v</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Recent press on set i’ve done. How can I improve</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yza5rfy8fwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1k5c6t9</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>proposing a magnetic experiment with temperature</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5c6t9/proposing_a_magnetic_experiment_with_temperature/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1k5c35y</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Opalescent</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5c35y</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1k5apak</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>OPI Bubble Bath</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5apak</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1k5agw7</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Can someone explain the ORLY drama?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5agw7/can_someone_explain_the_orly_drama/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1k5ad3j</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Press-On Pros: I could use Guidance on Longevity, Nail Health, and the Gorilla Glue Test (don’t judge me)</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5ad3j/presson_pros_i_could_use_guidance_on_longevity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1k5acbz</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>U magnet and bar</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5acbz/u_magnet_and_bar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1k5a35h</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Or am I just terrified of Emma Stone?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5a35h</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1k59nnp</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Not for me :-( - any suggestions for improvement?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xie7caiqqewe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1k5922x</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Why do we not talk about F.U.N. Lacquer?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5922x/why_do_we_not_talk_about_fun_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1k58rwt</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Not sure i love it?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/982j7lugkewe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1k58d23</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>QDTC pulling on cream polishes?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0mu680jhewe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1k589ec</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Tried to do a magnetic cat eye, but the pigments always seem to disperse :(</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1pywlhrgewe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1k57mr4</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Practicing fluid nail art on my ultra shorties! 💅</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k56imj</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1k57ikw</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Any recommendations for opaque neon nail polishes?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k57ikw/any_recommendations_for_opaque_neon_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1k5744e</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>My tiny wonders chose the same nail polish.</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkccxet28ewe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1k56pwb</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Sorry but what? This colour is insane 😭😭😭</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k56pwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1k53ldw</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Second home mani after a year of builder gel destroyed my nail beds!</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k53ldw</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1k535x8</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Pastels for Easter</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k535x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1k52ylk</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Today's haul :')</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx9iacxd5dwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1k519pz</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Essie Jelly line- help needed</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/electetujcwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1k5t6ab</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>My Stain Glass design vs Ais design</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5t6ab</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1k5nfhb</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Easter Break Set</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erygu110ohwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1k5lvib</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>The cats meow</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4bs2b4z9hwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1k5lmrf</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Summer press-on set 🐟</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5lmrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1k5ioet</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>minecraft art!!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5ioet</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1k5hoxw</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>'powdery' texture effect, questions!</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k5hoxw/powdery_texture_effect_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1k5h5wh</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Alitasnails did such a beautiful job on my birthday aura gel x set</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9y4rqccd8gwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1k5h5h7</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Opal Galaxies 🌌✨</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/og7y1rn48gwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1k5gxtf</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Very first set from a few months ago!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5gxtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1k5gevg</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Butterfly set</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5gevg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1k5f3ta</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Newest nail set</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ej8f907htfwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1k5frua</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Shoe Diva Frenchies 👠💄👗</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxln0l4ayfwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1k5fhzf</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Peeps Nails!</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5fhzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1k5eo7l</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Practice for the day 🦋</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5eo7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1k5e6ok</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Magical cats</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5e6ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1k5c8hq</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Classic ladybug butterfly naila</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/feav98w89fwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1k5b86o</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>new week, new set, same colour palette</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5b86o</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1k58y2m</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Moldy sea witch set</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k58y2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1k58xjl</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Easy peasy Coffee Nails</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/PW2qoN6GoNw?si=vGBvUpfabvRyjJAi</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1k564oe</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>My slightly-mismatched Peeps for Easter</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k564oe</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1k55rbq</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>When I feel like I haven’t progressed 😱😍</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wxdg22t4xdwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1k4vqiq</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Girls, my first 3D design inspired in Gloomy Bear</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ddnvp9itawe1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Apr 24 08:12:21 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_27.xlsx
+++ b/data/collected_data/2025_04_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C664"/>
+  <dimension ref="A1:C839"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11721,6 +11721,2981 @@
         </is>
       </c>
     </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1k6msq8</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Just finished this set of Gloomy Bear nails!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pug02pl6pqwe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1k6ml4n</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>I found my new favourite nail salon… my tech killed it!!</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1ax8djgmqwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1k6mbig</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>my second set of nails!!!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6mbig</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1k6li6l</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Should I be upset?</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6li6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1k6lh9n</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>When you love what you do, everything is done with love</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6lh9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1k6kkyc</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Hyper realistic pierced nails!</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6kkyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1k6kem8</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Tried some nail art. What do we think?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6kem8</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1k6kajh</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>My nails 🔥♥️🖤🩷💜</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6kajh</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1k6j9li</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Obsessed with the Manucurist Active line</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6j9li</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1k6j73u</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>My birthday nails!!! (nail tech: @naillsbynini on IG)</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6j73u</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1k6jqff</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>DIY press on nails question</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6jqff/diy_press_on_nails_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1k6j392</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>set my friend did for free</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6ga94w2ipwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1k6hl6i</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Color advice!</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6hl6i/color_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1k6j2cy</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Cutesttt nail press ons</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6j2cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1k6izxn</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>My new venture, do you like it?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xja9idr4hpwe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1k6ijfi</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Spring Mani ❤️</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6ijfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1k6icth</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Easter Set 🐰</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5mu98gvapwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1k6gchy</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>would putting wet acrylic on the natural nail then a full cover nail extension ON TOP of the acrylic and letting it harden kinda like gel x cause contact dermatitis ?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7z35glr6towe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1k6hzqp</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Tried something new</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6hzqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1k6hwz0</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>That sparkle✨️✨️</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vrxzdu4o6pwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1k6hv8c</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>We still love Chrome, right?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5kld5i4a6pwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1k6hqhu</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>My new set!!🍎🍏✨</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02tv1wrf5pwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1k6hmfs</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>First time getting Gel X</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6hmfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1k6hi7c</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Hard gel overlay on builder</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6hi7c/hard_gel_overlay_on_builder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1k6hbmq</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Subtle sparkle✨</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6lmovvl1pwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1k6h106</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>April showers ☁️💧🌱🏵</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6h106</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1k6gg8w</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>This weeks set :)</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6gg8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1k6g9qo</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>My New Set</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6g9qo</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1k6g3fu</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Nude chrome manicure 💅🏻</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg2gbkdyqowe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1k6fyhc</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Builder gel and shape tips needed</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6fyhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1k6fr42</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>I really looove this silver chrome, I'm obsessed</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rxc6w4lnowe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1k6fni5</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>I've finally mastered my gelx application 🎷🐛✨</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6fni5</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1k6fd3x</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>my sister’s nail work</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6fd3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1k6ebju</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Help me figure out what's wrong</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6ebju</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1k6egh3</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Potentially stupid question: do gel x tips need to be cured?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6egh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1k6dz48</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Um, what? Nail journey</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6dz48</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1k6dl3t</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Mindflayer Press-On Nails</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ohw9ix1w4owe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1k6difc</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Healing process</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6difc</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1k6e0ib</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Spring Nails!! 🌸🩷</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ry20gy5h8owe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1k6dv30</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Gel removal taking forever!</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6dv30/gel_removal_taking_forever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1k6dcga</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Is this the right neutral for me?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oa3244o91owe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1k6dbfa</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>this took me hours pleases be nice🥲</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h58yl7dp2owe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1k6cwu9</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Broke my finger and when it’s healed the skin has gone super far back how do i fix this??</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6cwu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1k6cy4b</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Strawberry nails! 🍓</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02vdkqopznwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1k6csfh</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6csfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1k6b9uz</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Tips for blending colors better?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6b9uz</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1k6cgjh</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>cat eye!</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92tj92kvvnwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1k6cev9</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>simple but perfect for my japan trip</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7nr8kghvnwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1k6c9qf</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Vacation nails</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xj953jadunwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1k6c7em</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Thin and weak nails</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6c7em/thin_and_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1k6c6q4</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>One of fav sets</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6c6q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1k6by5s</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>I haven’t bit my nails in over two months!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6by5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1k6blh0</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>My set from today!</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cxdpfq4pnwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1k6b4vr</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Love my wonky set</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6b4vr</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1k6am8a</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Ugh I suck at gel x</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rd94golthnwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1k6aokk</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>It's summer time so it's a best time for color change from red to pink 🤗</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1k4kz6ainwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1k6a2bj</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Made some press ons!!</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbaswxvsdnwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1k6ah1u</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Before and after</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6ah1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1k6aggw</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Some sweet little Mycenaean Suns to herald in the warmer weather ☀️</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6aggw</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1k6acrj</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>I’m in love with frogs</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwe3fvuwfnwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1k6abp6</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>New nails 🌈</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g29ypgxnfnwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1k6a97e</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Did my own birthday nails!</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yluqks7fnwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1k6a26c</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Nails Grows in Broken</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32d5ijdrdnwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1k6a0f0</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>✨🩵🤍💚🫧🎀Nails I got today did something brighter for spring time🌤️🌷&amp; got my toes to match, the 2nd picture is what I had before(red cat eye❣️🥀🖤- you can tell I love the cat eye look lol)🥰🫶</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6a0f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1k6976t</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>what do we think?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxaosx5f7nwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1k690vd</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>💜 mooncat Flight Of The Monarchs 🦋</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k690vd</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1k68v4s</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>do your nails mix up with your skin ?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k68v4s/do_your_nails_mix_up_with_your_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1k68uhu</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Something Cute💙❤️🩵🩷🤎</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k68uhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1k68rc3</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>yellow mellow 💛</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k73v0o8a4nwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1k68f58</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Jelly reptile vibes 🐊💙</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmdubl2s1nwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1k68asf</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1gxv05w0nwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1k67y1i</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Les gustan?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bj2rq77cymwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1k673gc</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>gel keeps cracking in the same spot on my thumb</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jrmdjh6smwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1k66vvc</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>🏳️‍⚧️ Showing off my Easter nails 🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k66vvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1k66aeh</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Just tried a new color combo!</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k66aeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1k65xqy</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>What do we think about these press ons ??</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tme3p7yjmwe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1k65u1f</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Spring Nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3j6avvr8jmwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1k65izs</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Simple, but cute for spring.</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4k8yif2hmwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1k65gdg</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Love these, though the rose snags on everything</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kjipyl7gmwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1k65d99</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k65d99/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1k6592c</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>How can I fix it? 😭</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44o2q0f4fmwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1k651ur</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Custom size press ons from KTNailArtStudio on Etsy</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7bq7xjodmwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1k64zhx</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Couple days late but my nail tech gave me the cutest Easter nails!</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k64zhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1k64otf</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Do I need to find a new nail salon? Day 8 gel manicure</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/esgb4g24bmwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1k64zat</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>First Time Trying Transfer Foil</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k64zat</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1k64vas</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Jelly nails🍷</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k64vas</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1k64spo</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Adore the pink white ombré</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0dyajxvbmwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1k64mnf</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Tried doing cat eye for the first time, would love feedback</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v4ps9mpamwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1k64lm8</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Can't wait to wear this color again</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8svc4rqhamwe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1k6297o</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Recommendations</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6297o/recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1k630o1</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Took me 2 business days to do…but I’m really happy with how this set turned out!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k630o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1k635qf</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Dip powder vs press-ons</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k635qf/dip_powder_vs_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1k647ay</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>What to do for broken nail?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yy6rr6rp7mwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1k649rk</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Gel nails</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcdpb7q78mwe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1k641lg</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Ombré 🧡🩷💜</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbyjt25k6mwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1k63jly</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>First time French</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yz73dzsw2mwe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1k63j86</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Part of lunula is missing</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdp5m3ct2mwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1k63hi6</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Show me your favorite nail set you've had!</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k63hi6</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1k63d2n</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>3D Nail Art</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k63d2n/3d_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1k62ttv</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k62ttv</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1k6j9xn</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Holo Taco Coral Chaser during golden hour</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/giyhwlpxjpwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1k6l0h7</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce - Dirty Margarita</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6l0h7</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1k6jxjt</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Looking for a similar color from a discontinued brand</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k6jxjt/looking_for_a_similar_color_from_a_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1k6ilkf</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Half blue/Half pink (BLUE RIZZLER / POP ROCKER)</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6ilkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1k6iepn</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>sassy sauce brush?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k6iepn/sassy_sauce_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1k6i5k9</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Does anyone have a rec for very subtle rainbow topper — either small glitter or holo — that could go over a white base? (wanting to match moissanite stone)</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k6i5k9/does_anyone_have_a_rec_for_very_subtle_rainbow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1k6gusn</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Paint it pretty on Instagram: "Something’s dropping… but what is it? Follow the trail to find out who else is in! @prairiecrocuspolish We’re spilling the details on April 25</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DIzvfsIPi2A/?igsh=MWxtamhqMDlvdG1iZQ==</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1k6fts8</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>There Is A Glitz In The Matrix💜💙</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6fts8</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1k6f2gk</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Marsala Jelly on short nails! I thought I hated the hated working with jelly polish, turns out I just hate the brush this comes with. Swapped it out and finally got the even results I’ve been hoping for.</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6f2gk</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1k6etd0</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Gold Leaf Fingers!</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6etd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1k6eil8</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>canNOT stop smelling my finger!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1j5gvi4ccowe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1k6dmbb</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Who needs expensive studio lighting when you have a work bathroom?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6dmbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1k6dcbi</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>I think I'm getting the hang of velvet?</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hdbe2guu2owe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1k6cq5c</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Arcana Lacquer - Tropicorn</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6cq5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1k6ckbx</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Flower confetti dupe?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6ckbx</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1k6cbmh</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>My natural long nails</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjcpiugrunwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1k6bqag</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Dupe for this polish?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6bqag</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1k6bmju</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>LynB haul arrived!</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6bmju</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1k6asj2</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Travel containers for liquids</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k6asj2/travel_containers_for_liquids/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1k6acys</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Butterfly nails</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6acys</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1k6a7zw</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Giving a chance to the polishes I barely use/don't like...</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6a7zw</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1k68yl4</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Dreamland Lacquer Date Night.</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1lvzwgp5nwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1k68ye7</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>💜 mooncat Flight Of The Monarchs 🦋</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k68ye7</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1k68w92</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - question</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k68w92/lurid_lacquer_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1k68u2v</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>OPI RapiDry is *not* it.</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3epevzct4nwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1k68twc</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Spring Day</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mrbmkjo4nwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1k68kis</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Found on Pinterest, Color ID Req</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6xkk61w2nwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1k66dfs</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>My first real attempt at art! 🐟</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k66dfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1k65u8q</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Ultra holo in the sunlight 🤌🏻</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k65u8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1k65loj</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Magnetic Skittle</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f4pvrenlhmwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1k65kfk</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Scope It Out🔬</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gqvkvfjchmwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1k65imw</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>When you’re unhappy with your current mani…</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aszbaztzgmwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1k65bb0</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Thank you’s and question</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k65bb0/thank_yous_and_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1k64oc4</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>dreamscape ✨</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k64oc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1k64mlg</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>How to cover/secure nail tears - silk wrap + dip powder</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k64mlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1k64h9u</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Don’t sleep on Walmart!!</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k64h9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1k64gvh</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Velvet tips 🔮🪲🦚🦜</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rw30grmj9mwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1k641rl</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Tips for using at home glue for press on nails</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k641rl/tips_for_using_at_home_glue_for_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1k62mul</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>You all know and love her. Now, so do I.</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aqx0m5bbwlwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1k62ljr</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>In Love with this Color 🥰</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k61sxl07wlwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1k62fas</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Killing time at the airport but at least I can get distracted by shifty nails</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k62fas</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1k62b39</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Has anyone tried Flora1761?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx8pxgs3ulwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1k61zx5</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Late Easter mani submission</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04dle40vrlwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1k61yin</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>How to address nails with heavy grooves?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k61yin/how_to_address_nails_with_heavy_grooves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1k60oxi</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>New week, new colour</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k60oxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1k60h9a</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Normalizing imperfection!</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k60h9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1k5zf5r</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Rough start to the day 😭</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5zf5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1k5zese</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Easter/Spring Nails!</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5zese</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1k5z9tb</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Mooncat Base Coat</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5z9tb/mooncat_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1k5yn4w</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>I’m so proud of this - shaping efforts</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5yn4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1k5y30u</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>holy holo 🤩</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5y30u</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1k5xlrw</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Back again with another great green set. ILNP Olive Grove</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5xlrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1k5ve9d</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Velveteen</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5ve9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1k5l6i4</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>White chrome help</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnctawh04hwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1k5uidq</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Best non-glossy ridge filler for men?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k5uidq/best_nonglossy_ridge_filler_for_men/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1k5ufwg</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>I didn't think I would love this color this much</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5363i5cvtjwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1k6mxji</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Just started doing my own nails</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6mxji</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1k6jf56</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>chekered nails</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7uk4woglpwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1k6i2ik</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>tried doing ombre nails myself! tips to improve</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzk6jgl48pwe1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1k6g2gw</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Both of the Art History sets on my hands</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/if1kbi3lqowe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1k6g0xl</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Organic pink</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6g0xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1k6c0lw</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Shimmy shiny</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bp6p0u5asnwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1k6af5j</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>3D aura nails</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc1utoldgnwe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1k6adxg</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Fourth wing inspired nails 🥹🖤 I worked so hard on these</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scize785gnwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1k69yro</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k69yro</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1k69r3e</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Blue Sunflowers</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k69r3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1k69hwr</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Been doing my nails evey so often</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k69hwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1k67wtz</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>¡¡¡ Stones, Hearts and Browns !!!</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k67wtz/stones_hearts_and_browns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1k67idq</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>🌸Came up with some Springtime Nail Designs Using Up Older Colors</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k67idq</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1k673fg</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>I can’t decide</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k673fg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1k63qbw</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Custom press on nails with 3D sculpted dogs</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k63qbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1k613p4</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>For Star Wars Night at Disneyland ✨</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ljsbdhfllwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1k5xyxd</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Floral Illusion Nails</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8az0oxegwkwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1k5vnzp</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Took me 2½ hours and I didn't even do my right hand...</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k5vnzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1k5n4xa</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Nail technique for prom manicure</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0ww4e3blhwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Apr 25 08:12:19 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_27.xlsx
+++ b/data/collected_data/2025_04_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C839"/>
+  <dimension ref="A1:C1021"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14696,6 +14696,3100 @@
         </is>
       </c>
     </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1k7fgz8</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>I think of the ocean.</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqguznibtxwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1k7ev1u</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Any other shape that would look nice ?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahikqahdlxwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1k7eti4</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Are these ok</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7eti4</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1k7esz4</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Is the Barbie "Doll'd Up Nails" a good product in 2025? Or any recommondations?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmwz2muikxwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1k7e683</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Cuccio cuticle oil drying me out</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6na687qrcxwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1k7e3mw</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Progress?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7e3mw</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1k7dw4r</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>I wanted transparent gel. Maybe it's better this way. Transparent gel and pink finish, over natural nail</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7dw4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1k7dqa8</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>My nail tech did me so good</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkjie8im7xwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1k7dml4</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>a little rhinestone action ✨</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/loxk8hwd6xwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1k7dman</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Clouds in the clouds ☁️</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7dman</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1k7dil8</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Pink mani/ pedi</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7dil8</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1k7dh8g</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Short mani</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7dh8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1k7a73c</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Does my natural nails look damage? They were very bendy so I cut it off. Been trying to do builder gel but it didnt work and kept lifting 😭</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7a73c</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1k7a1vp</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>new to acrylic…help a girly out!!</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7a1vp/new_to_acrylichelp_a_girly_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1k79gbx</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Tried builder gel for the first time. How did they do?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/sxs2lKB</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1k78wog</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>help with choosing colours for an american mani</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k78wog/help_with_choosing_colours_for_an_american_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1k76poy</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>New to acrylic…help a girl out!</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k76poy/new_to_acrylichelp_a_girl_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1k7ckun</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Gel builder</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0m50kwdluwwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1k7d60x</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Today’s nails</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7d60x</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1k7bngu</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>If I break a nail do I have to pay for a full set or can I ask for a fill</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uv9hz225lwwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1k7aw8d</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>strawberries for spring 🍓</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9t16l43qdwwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1k7ats6</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>🤩</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akeynn12dwwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1k7aj60</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Help needed. No idea where to start.</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7aj60/help_needed_no_idea_where_to_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1k7afba</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Madam Glam storage 🤔</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxeesjn79wwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1k79tc3</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>The weirdest nails I’ve ever created🎣🐟🐠🐡</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqhd4exj3wwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1k79lns</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>First time with dip</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ju37som1wwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1k78ywm</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Guys painting their nails</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k78ywm/guys_painting_their_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1k78bks</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>My friends nails for stage coach ! Did these with builder gel</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zajru6gupvwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1k789vz</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Birthday nails 🥰</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ihvm54yepvwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1k78653</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Damaged nails</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k78653/damaged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1k782bo</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Black tips</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k782bo</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1k780g8</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Pink nails</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k780g8</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1k77q36</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>What do we think, i tried something new 🙈</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyd0u0cgkvwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1k77pyo</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Looking for some kind of box/organiser</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k77pyo/looking_for_some_kind_of_boxorganiser/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1k77pip</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Trashy, dorm-done, mental breakdown, shroom trip nails.</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k77pip</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1k76jh3</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>I've always had soft and bendy nails, how do I fix that to make them harder?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k76jh3/ive_always_had_soft_and_bendy_nails_how_do_i_fix/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1k76rs2</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Mismatched japanese inspired nail designs</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k76rs2</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1k76u28</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>in love with this colour</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccfgybrqcvwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1k76nt7</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Biab</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k76nt7/biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1k76fih</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Fresh set!! It’s been so long, I missed my claws &lt;3</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k76fih</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1k76204</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>I couldn't settle on one color combo, which is your fave?</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k76204</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1k75woa</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Soooo happy with this set !</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vvybpzt4vwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1k75awn</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>OPI “Intelli-gel” gel polish</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k75awn/opi_intelligel_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1k75okw</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Encapsulated rose 🌷</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rc3r9vr1vwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1k75df8</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Thoughts on this color?? DND Diamond Eyes. It’s a bit more “electric blue” than I thought it would be!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ls2sq6vf0vwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1k752t6</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>I got Snoopy nails 💕</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50drcmo1yuwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1k74z1c</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Funky new set!</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k74z1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1k74igt</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>First nails I did myself in years without a professional. Looks good?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2pfhe10tuwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1k742zz</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>In a pinch - can I use superglue?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k742zz/in_a_pinch_can_i_use_superglue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1k73ktd</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>🤎🧸🍫🍷</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gz4ensxbmuwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1k73hra</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>I forgot to show my first design of the year 🎀🩷</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7he7lncoluwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1k73gu3</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>For the first time ever I have healthy strong nails!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k73gu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1k73g13</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>I AM SO PROUD</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k73g13</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1k72uj7</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Miami Vice</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fb78lqsuguwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1k72t56</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>My nail tech is always crushing it.</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k72t56</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1k72j0d</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>question</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k72j0d/question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1k72cqd</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Idk how it happened</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k72cqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1k726fn</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Nails inspired by u/lindeebean</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k726fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1k723s9</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>So much progress ✨️</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k723s9</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1k71lvs</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Should I get these fixed…?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k71lvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1k71ch8</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Black and white set</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k71ch8</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1k70is0</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Grungy Nails</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k70is0</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1k70dgp</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Recent Manicure!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iljpf66wytwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1k704nv</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Porcelain nails</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k704nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1k6zuu7</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>New to DIY press on art</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6zuu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1k6zezc</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Is the gel paint easier than gel polish?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6zezc/is_the_gel_paint_easier_than_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1k6z3dg</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Any NYC girlies who get tips?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6z3dg/any_nyc_girlies_who_get_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1k6z2x9</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>How can I help my nails?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4xkynllptwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1k6z917</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>the perfect combo 🤍</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/busvqfcsqtwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1k6z71i</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Red nails anyone?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6z71i</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1k6yj6o</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>My attempt at the jelly nails.</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ya6xp1eqltwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1k6xgw3</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>First time getting nails done do they look terrible</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6xgw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1k6y6or</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Does this look like raw chicken??</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0xydjj8jtwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1k6ydgb</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Olive green</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2uxpq3lktwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1k6y9qy</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Beginner acrylic question</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6y9qy</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1k6y9d2</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>I was gonna buy myself flowers but decided to make some instead ☺️</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6y9d2</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1k6xldn</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Orquídea press-ons!</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49um42lxetwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1k6xhqo</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>My new extra orange nails</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34q6acn7etwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1k6xbl4</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>What nail color with this dress?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqv8i6z0dtwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1k6t4g1</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>short nail appreciation post✨</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drg4otpdiswe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1k6wy2b</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Fresh nude set</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eltsjn5catwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1k6wlzb</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Neon!</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqlcir0w7twe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1k6wjqg</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Yoshi nails! 💚🤩</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6wjqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1k6wj4x</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Neon nails go great with neon dinos</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp85re0b7twe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1k6w0a6</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>I'm so happy with these. What do you think???</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9wtnal5l3twe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1k6vvd4</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Idk what color to paint my nails , give some ideas</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6vvd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1k6vqww</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Going from long to short acrylics?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6vqww/going_from_long_to_short_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1k6tq6a</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>How often do you do your nails?</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6tq6a/how_often_do_you_do_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1k6ntvo</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Can you get the glossy look of jelly nails without using gel?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6ntvo/can_you_get_the_glossy_look_of_jelly_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1k6oug0</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Pop art on your nails: eyes, hands and hearts for a playful and bold vibe</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6ns7vccfrwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1k6pb1s</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>How do I remove nail glue from under the nail?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ht2l79pmkrwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1k6pu1f</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Can anyone explain how these things work?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iz1wp9p0qrwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1k6rl1y</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Home mani four months into growing out builder gel damage... 4.5/10 application, 10/10 satisfaction 💖😤</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvla3kpd6swe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1k6s8s9</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>can i use cheap on top of expensive??</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k6s8s9/can_i_use_cheap_on_top_of_expensive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1k6sami</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>💜🧞She Tried Her Best: Cat Eye + Chrome on Natural Nails (2nd Ever Set!)</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6sami</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1k6uu86</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Subtle silver 🤍🩶</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6uu86</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1k6twfy</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>I’m obsessed with my newest set 🦋.</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgkb64vdoswe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1k6ts3z</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Simple but I loved them</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnkxtlahnswe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1k6tee1</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Fresh set on myself</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6tee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1k6t3vh</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Does it look elegant, basic… or what do you think?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gb6nh9reiswe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1k7e455</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Looking for my new holy grail, cruelty free QDTC</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7e455/looking_for_my_new_holy_grail_cruelty_free_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1k7dxea</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Three Sisters of Lake Superior (LynBDesigns)</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7dxea</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1k7d16y</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Glass nail file - can this be taken as carry-on ?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7d16y/glass_nail_file_can_this_be_taken_as_carryon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1k7clo0</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Choice paralysis</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7clo0/choice_paralysis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1k7azos</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Slowly making my nails more pointy…..</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7azos</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1k7axb7</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>What is a gel-x fill and why do salons push this instead of a new full set?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7axb7/what_is_a_gelx_fill_and_why_do_salons_push_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1k79y4e</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>polish thinner recs?</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k79y4e/polish_thinner_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1k797vv</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Did my own wedding nails! 💅🏻</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdav90y2yvwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1k794vb</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Chrome sweet chrome</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k794vb</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1k78w5y</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Been stressed and nail bitey while wedding planning so I grabbed some new polish. Lord Vader is STUNNING</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qm16ktz2vvwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1k78ixw</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>help with choosing colours for an american mani</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k78ixw/help_with_choosing_colours_for_an_american_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1k786qi</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Sandy Cracks 🤩 (sun, cloud, and artificial light)</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k786qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1k7802p</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Emily de Molly sale?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7802p/emily_de_molly_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1k77ehb</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>big chop anyone?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k77ehb</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1k7756o</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Eternal Forces 💜✨️</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7756o</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1k76xrb</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Heartbreak</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k76xrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1k769hv</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Had to buy it after seeing it on here last week</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/94vsjegq7vwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1k763br</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Mooncat’s Devil’s Ivy</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4m3ih46b6vwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1k74t5e</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>What’s this in my base coat?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k74t5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1k74npn</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Spring nails or fashionably late easter nails</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zajzzjppuuwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1k74cxi</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Galaxy nails! 💅 🌌</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n80z1uxbsuwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1k74bx7</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>This combo is so Dreamy</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k74bx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1k7434c</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Essie The Girl$ Are Out vs Pencil Me In</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7434c</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1k73exq</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Can Structured Gel Soak Off</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k73exq/can_structured_gel_soak_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1k735si</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Possible Prugly?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k735si</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1k734w1</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Trying pebble jelly nails with regular polish</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k734w1</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1k72f0g</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>practicing🙌🏼🙌🏼🙌🏼 in my new venture, do you like them?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/faskzvloduwe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1k727r1</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Apocalypse Polish Haul</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k727r1</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1k6v99b</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Holo Taco Thyme After Thyme + Garden Party - natural and flash lighting!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kyf7e218yswe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1k6ww7o</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>The perfect nude for my skin tone 🤓💅🏼🩷</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4v3ga5z9twe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1k70let</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>This nude isn’t quite right. Any recommendations?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k70let</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1k6zhud</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Lemming Lacquers Brigid is GORGEOUSSS😻😻</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgdv75djstwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1k6zcqd</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Mooncat Obsession</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6zcqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1k6za3g</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Converted by this ugly cute thermal!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6za3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1k6z9i0</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Multichrome French Mani ✨</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pwq69bcwqtwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1k6z919</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Dupe for MC The Stranger??</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6z8du</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1k6y0rl</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>took this subs advice and got stronger magnets</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rpikc912itwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1k6xoeg</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Had to do a lil skittle to christen my first Holo Taco polishes!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6xoeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1k6xah3</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>If frogs had wings</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0u9tfwsctwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1k6wzt6</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>a mani most strange, kinda love it though! a $14 lacquer and a $0.98 one 🤌🏼</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6wzt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1k6wr7k</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>ILNP Enchantment</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnc6ry2z8twe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1k6wmtu</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Lost a polish,looking for dupe +Vent</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6wmtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1k6vieg</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Mooncat musts</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k6vieg/mooncat_musts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1k6va4o</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Isle Be There by KBShimmer</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4arb6beyswe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1k6ujvs</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Not very Spring of me!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6ujvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1k6twe0</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Freehand nail art for spring 🍓🫐🍇</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6twe0</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1k6tb0f</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Moon cat Forbidden Fruit</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6tb0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1k6szyk</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Saying no spring manis ❌</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6szyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1k6s7xa</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Finally thermal weather</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6s7xa</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1k6s42y</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Help Finding a Similar Shade</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6s42y</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1k6s1qo</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Happy 1 year anniversary Arcana Lacquer!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6s1qo</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1k6rvv4</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Classic Red</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/iKhIzTT</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1k6rnrn</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Please show me Born Pretty Iridescent Glass Blue with different magnet patterns</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k6rnrn/please_show_me_born_pretty_iridescent_glass_blue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1k6rmds</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Baja Blast dupe? 👀</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6rmds</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1k6rlwn</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>A moment of silence🥲</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnecocrk6swe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1k6r6kl</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Springtime sparkles!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6r6kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1k7dksa</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Clouds in the clouds</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7dksa</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1k7b1xu</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>First post! Made these for a friends anniversary. First press ons for someone besides myself &amp; First set I am 100% happy with! 😊</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7b1xu</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1k7b1l2</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>I love this color, what season would this be best for?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7b1l2</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1k7ara6</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>pls WHY IS CAT EYE SO HARD TO FIGURE OUT 😩</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k7ara6/pls_why_is_cat_eye_so_hard_to_figure_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1k77y69</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Bubble Nails ...</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k77y69</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1k76xqh</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Practicing my lines</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k76xqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1k75f76</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>I’ve been trying my hand @ making my own press ons. This is my third ever set. Any tips?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umde9ugc0vwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1k74v22</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Swan nails✨🦢</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k74v22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1k72ebu</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>MPA pallet versus DGEL paint pods??</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k72ebu/mpa_pallet_versus_dgel_paint_pods/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1k71xlj</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>mcbling meets gyaru nails</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k71xlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1k71x97</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>How do i improve? been doing it like this forever</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnldblru9uwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1k71g6q</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Black and white</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k71g6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1k70exc</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>red aura 💅</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0nxpzbg6ztwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1k7044n</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Gel and nail art</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7044n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1k700ge</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>soft gel cat eye 🐈</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k700ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1k7001w</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>frutiger metro nails by amazing friend! @micenails on ig</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3caswq7wtwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1k6zpvt</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Practicing. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rf2ixux6utwe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1k6xzid</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Tried Kimi No Nawa nail art :)</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nzjz86vshtwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1k6whg7</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Alien egg nails inspired by glass beadwork</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvo2dbqy6twe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1k6vmjz</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>practicing🙌🏼🙌🏼🙌🏼 in my new venture, do you like them?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nn56rpxw0twe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1k6vehr</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Cake nails with a vintage twist (I don't dare call them vintage cake nails haha they dont really look like it)</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/khmx7ndczswe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1k6u222</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Nails for my mother in law’s wedding</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7xsirxjpswe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1k6rw2s</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>hiii how do i make these kinda wavy nail art? what gel do i use?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o51blg9x8swe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1k6qg9m</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>I'm learning</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4ataq541wrwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1k6pxbn</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Can anyone explain how these things work?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hprlfuzvqrwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1k6pwbw</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Garden of Eden inspired nails</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k6pwbw</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Apr 26 08:10:20 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_27.xlsx
+++ b/data/collected_data/2025_04_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1021"/>
+  <dimension ref="A1:C1199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17790,6 +17790,3032 @@
         </is>
       </c>
     </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1k86j5e</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>First time working with charms!</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k86j5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1k8730x</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>For all my red lovers ❣️</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8730x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1k86hu6</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>New press ons 💖💖💖</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ic0r5dii4xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1k860wu</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>My melody press ons</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2424kc34d4xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1k85y6s</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>SOS - Mechanic who’s new to extensions!</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k85y6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1k85uno</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>First time doing gel</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uva8lzh5b4xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1k85qnw</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>I know they're not perfect but I love them so much</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzbz6hqu94xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1k85gwe</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Dazzle dry</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddmddwiq64xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1k85g6z</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Missing a finger and have always wondered this …..</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k85g6z/missing_a_finger_and_have_always_wondered_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1k856o4</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>First professional mani+pedi</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k856o4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1k84mbo</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>New set; Pompompurin and Macaroon!</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avzowb82x3xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1k82myj</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Pain in my nail</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k82myj/pain_in_my_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1k83zpr</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>I love how they turned out</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhrxlb0kq3xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1k83lfz</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>What to use to disinfect a foot spa?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k83lfz/what_to_use_to_disinfect_a_foot_spa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1k83bek</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>First Time DIY Polygel</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k83bek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1k83456</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>New chrome nails</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k83456</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1k82i6r</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Ideas for nails that would complement the ring?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vi8z5g3wb3xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1k82cjp</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Store bought but I thought they looked so cute!</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvgjo6aea3xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1k81xlv</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>New (short) Nails!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17hhfqtc63xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1k81wkt</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hl14cfc363xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1k81s8z</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>You like it? I LOVE IT!!!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvszl8gw43xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1k81joj</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>What shape are my nails and what shape would look best on me?</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k81joj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1k81gbl</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>At home mani. Do the color and/or shape suit me?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qnhc69o13xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1k81eng</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>If you were gonna make a list of things a noob would need to just start doing there own nails (gel x or acrylic)</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k81eng/if_you_were_gonna_make_a_list_of_things_a_noob/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1k813a2</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Could I use a nail art pen to colour in my nails before applying more gel polish on top?</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k813a2/could_i_use_a_nail_art_pen_to_colour_in_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1k80tq9</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfzh4bdtv2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1k80t63</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>April Nails</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbfewxinv2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1k7zv72</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>How do I start doing my own?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7zv72/how_do_i_start_doing_my_own/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1k80lsw</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Product recommendations</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k80lsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1k802fr</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>This Neon Green is giving me Spring Vibes 💚🍀</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwj3huaro2xe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1k7zvyf</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Nail Drill Recs</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7zvyf/nail_drill_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1k7zups</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>First time doing sculptured nails !</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7zups</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1k7zc52</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>My natural nails now vs how they were in November</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7zc52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1k7zdvx</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Obsessed with this marble design!! Marble nails, yes or no?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4cipneji2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1k7zdgz</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>New set ♥️🐆✨</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rk7nicimi2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1k7zb49</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Breaking out the bright colors again!</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqpj1322i2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1k7ysqu</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>The process 🌈🌸</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eynkbewbd2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1k7yqgi</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Colorful crocodile set for spring</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7yqgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1k7yhgg</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Red French Tip Ombré</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmx5alvva2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1k7ygoj</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Latest set! Apex tips, nail foil, and gold flakes!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yz0jxpipa2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1k7xas5</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Getting my nails done after 2 years!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxghr5l212xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1k7x5y7</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>What do we think of these?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpnjkxmyz1xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1k7wxqi</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Pink French nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8t54gbe5y1xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1k7ww39</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Fresh set for May ✨️</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2rq0m6tx1xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1k7wqpe</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Cowboy carter nails!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7wqpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1k7wdi1</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>New to Manicures</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7wdi1/new_to_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1k7w883</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>In love with this color. Added a cursed pose for fun.</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7w883</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1k7vwq2</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>First time getting my nails done. I’m obsessed 🍒</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7vwq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1k7vvdd</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>A set im really proud of 💖</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7vvdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1k7v9ci</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>What's going on with my nails?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7v9ci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1k7ugz8</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Tried press on nails for the first time from Kmart- what is the best way to remove them without damage</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7ugz8/tried_press_on_nails_for_the_first_time_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1k7un81</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Olive &amp; June</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7un81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1k7uasg</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Are electric nail files the only way to file/buff your nails and do cuticle prep?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgbg2sj0e1xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1k7u4eo</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Wedding trial nails</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7u4eo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1k7u142</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Pink Bunnies 🩷✨</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/155a02qsb1xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1k7tk4j</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>So excited to finally try this color</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vmalvje81xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1k7tppm</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Spring/easter nails for $45!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhkxykok91xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1k7tie3</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>☀️ natural look</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnktb1t181xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1k7tgx2</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Gel, acrylic or dip?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7tgx2/gel_acrylic_or_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1k7tghq</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Disappointed in my nail art</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7tghq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1k7tg5m</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>How much would you pay for this set?🩵</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5jiay7nk71xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1k7ssfn</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Did my nails after a while. Strawberry jelly cat eye + french chrome</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzbiaual21xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1k7spuk</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Do you notice when other people have grown out cuticles?</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7spuk/do_you_notice_when_other_people_have_grown_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1k7sky0</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>First time in a long time getting my nails done and First time doing almond! They came out so cute And using my dogs fur for the back ground lol 😆</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4z2t4k111xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1k7sj7k</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Nails 😍 (I couldn't decide on a color, so sorry if the colors I chose look a bit weird ☺️)</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7sj7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1k7sgbu</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Is this flattering on my hands?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7sgbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1k7rk3w</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Fake nail bubbles</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkq1ux5it0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1k7s0o4</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Really proud of how these turned out! 🥝🥝🥝</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7s0o4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1k7ru30</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>How many infills can I get</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7ru30/how_many_infills_can_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1k7rly3</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Nail salon Etiquette</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7rly3/nail_salon_etiquette/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1k7r7dh</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Removal issue or application issue? Are these rings of fire?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsr8c592r0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1k7f3xo</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>What to do with these nails??</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq1pabaloxwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1k7h4tg</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Builder Gel keeps peeling off - need advice!</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s64fdnmqeywe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1k7hwom</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>How damaged are my nails?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7hwom</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1k7jdga</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Kingsday nails are done!</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7jdga</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1k7oywu</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Nail gods and goddesses - what the heck is this</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0owh3cra0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1k7ql4m</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>My coworker does my other coworker’s nails every week. Here are this week’s.</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tj12hb4jm0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1k7ps70</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Proud of my work!</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulsj92vpg0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1k7qgke</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Mexican art inspired</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7qgke</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1k7qdx9</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>KBShimmer - Get Your Knit Together</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpanvl43l0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1k7qb2k</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Index fingernail is cracked (gel mani over natural nail) going to salon today or tomorrow…how will they fix this???</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7qb2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1k7q37c</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Went for an all different design on each nail! What do y’all think what would y’all change??</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqkbxj4wi0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1k7py3a</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Sticker gel nails</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7py3a/sticker_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1k7pvxv</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Deep round French</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9gjd8dhh0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1k7pqs4</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Rounded Nails</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7pqs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1k7plyo</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Drill Bit for Cuticle Care</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7plyo/drill_bit_for_cuticle_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1k7pbi2</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>A lil treat for myself</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7pbi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1k7p82g</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>What is wrong with my nails? :(</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pxm06xkc0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1k7p5bm</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Flash on/Flash off 📸</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7p5bm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1k7op6m</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>First time using builder gel:</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgcrr6lr80xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1k7ofxy</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Ombré Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/olrm1zzu60xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1k7o7f1</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Peel off Base On Top Of Hard Gel?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7o7f1/peel_off_base_on_top_of_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1k7o2y8</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Spring time nails</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7o2y8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1k7naeg</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>New ones 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/poeiw9uayzwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1k7n9n8</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Always end up going back to a nude ✨💅🏼</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7n9n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1k7n73i</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Shellac set looks so unprofessional. Should I complain?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7n73i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1k7klzx</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>BIAB Growth (4 months)</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7klzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1k7kgm0</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>can i mix 2 brands?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k7kgm0/can_i_mix_2_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1k7kftx</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>I traveled to Thailand for 2 weeks and went to a nails shop there</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfqu83z8czwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1k7k3lz</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Easter bunny</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/az6lqa5d9zwe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1k87thv</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>When you want to try the new magnet trick but fail to read product size properly</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6ba8oury4xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1k86anr</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Nail polish getting wrinkled with top coat?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k86anr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1k86793</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Weird color match question</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k86793</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1k857iz</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Sassy Sauce referral plz n ty 🙏❤️</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k857iz/sassy_sauce_referral_plz_n_ty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1k857h4</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Essie-Orchid Jelly is actually a crelly… mwahp-mwahp :(</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elymvazn34xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1k84qod</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Happy green to gold skittle</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gez652pgy3xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1k84lri</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Looking for the right brown polish</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k84lri/looking_for_the_right_brown_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1k835w0</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Cloud nails! ⛅️</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k835w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1k8324n</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I saw this on tik tok and screamed</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8324n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1k81z14</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Mooncat La Petite Mort Issue</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k81z14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1k818zj</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>ILNP FunHouse</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abjv5o9rz2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1k8081r</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Mariposa Mirror Effect separating on my nails?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/738r3hg6q2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1k7z3p6</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Loving BKL’s I Am an Appetite</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f4tfoblag2xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1k7yk5s</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>What to layer with jellies for best effect?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7yk5s/what_to_layer_with_jellies_for_best_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1k7yah0</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Desaturated jellies/crellies?</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7s3b33c92xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1k7xum3</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Cracked/ Glisten and Glow sale ?</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7xum3/cracked_glisten_and_glow_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1k7xsgo</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>rip</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7xsgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1k7xphf</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Concert prep</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/DJxtoeI.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1k7xn58</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Any good dupes for Polished For Days' shade "Moonwake"?</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7xn58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1k7xb8p</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Finally swatched my collection!</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7xb8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1k7xai9</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Rage Bait ☺️</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njkdgw8012xe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1k7x8o0</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Pearl-y Goodness</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1e4sf94h02xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1k7wewj</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>boring nudies with sneaky flakies✨</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2c5i0u1u1xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1k7w52f</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Are these three Sassy sauce shades super similar?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2t93nxf0s1xe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1k7vove</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Mooncat - To All Who Ghosted Me</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7vnz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1k7ums2</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Tips to clear up staining?</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zm903i8ig1xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1k7ultb</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>7 weeks on from my gels…</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7ultb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1k7uisq</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Playing with layers</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7uisq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1k7ugv0</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Does anyone use a Polyvinyl Butyral base coat OVER another base coat with any success?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7ugv0/does_anyone_use_a_polyvinyl_butyral_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1k7sea4</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Looking for polish similar to Mooncat Earth to Gaia</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7sea4/looking_for_polish_similar_to_mooncat_earth_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1k7sdf4</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Clionadh Mystery Bundle and Bday Haul</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7sdf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1k7s9h1</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Sunny floral accent thumb</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7s9h1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1k7s6vn</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Salt Water(Melon) Taffy - Clionadh Cosmetics</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7s6vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1k7s260</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>The purple trend continues!</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l30itee6x0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1k7rvxk</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Top Coat Recommendations</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7rvxk/top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1k7r2ge</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>apparition</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7r2ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1k7qv6r</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Does anyone like a nice pearl?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ddbdpujo0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1k7qhgn</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Best peel off base coat?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7qhgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1k7qe63</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>KBShimmer - Get Your Knit Together</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6ijo8u4l0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1k7q87o</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Pink and sparkly</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pt2bdtbxj0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1k7psdl</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Before and after - trip edition 🙈</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7psdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1k7pl7n</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Mani I did to convince myself not to buy more polishes</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krpn0oj9f0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1k7pgyx</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>VERY MUCH a first world problem, I know…</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7pgyx/very_much_a_first_world_problem_i_know/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1k7p466</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Most Flexible Nail Glue?</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pd7ij0otb0xe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1k7p3q8</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Mooncat Star Destroyer in honor of Andor S2</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eopr7dwpb0xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1k7ou0j</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>I heard old meme templates are back.</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7ou0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1k7o6yp</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Barbie pink💖</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7o6yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1k7o111</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Help me find a polish in this shade!</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/koehdnjs30xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1k7ngso</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>FUN Lacquer - Insomniac</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7ngso</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1k7mzi3</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Favorite top coat?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7mzi3/favorite_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1k7mw5m</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Essie gel setter top coat dries foggy</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfbiniedvzwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1k7mkuj</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>PPU timeline question</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7mkuj/ppu_timeline_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1k7leve</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>My first thermal!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7leve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1k7l8z7</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Chrome powder cracking</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7l8z7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1k7kpnx</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Matching Manis with Dice 💅🎲</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kl4ovsdlezwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1k7kiw7</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Salamándra 🔥</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7kiw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1k7jkqx</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>So Yellow flake, Green flake...1 2 3??</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7jkqx/so_yellow_flake_green_flake1_2_3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1k7idgp</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Does nail glue damage nails?</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7idgp/does_nail_glue_damage_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1k7gqav</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Comparison help - HT Lost in the Woods vs ILNP Park Ave</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7gqav/comparison_help_ht_lost_in_the_woods_vs_ilnp_park/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1k7bnpf</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>What’s Up Nails - Sale/Discount?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7bnpf/whats_up_nails_salediscount/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1k7d4dq</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Recs for one and done sheer with shimmer?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k7d4dq/recs_for_one_and_done_sheer_with_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1k82zoh</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>My third set so far ❤️</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k82zoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1k81u6c</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Couldn't decide if I wanted negative space in my stained glass nails</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k81u6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1k7zwrx</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Working on my realistic flowers 💐</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7zwrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1k7z2qm</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Spirited Away nails. I think I'm getting better!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7z2qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1k7yiz1</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Graphic Art Cherries</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbb2cm39b2xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1k7ut6a</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Pink Bunnies 🩷🐰✨</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oet0f7esh1xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1k7te91</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Nail "code"? Why do many sets have different colours on two nails?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k7te91/nail_code_why_do_many_sets_have_different_colours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1k7qpd8</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>¡¡¡ French cowgirl !!!</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k7qpd8/french_cowgirl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1k7qiti</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Any idea if this type of effect can be achieved with gel polish or it’s just an unrealistic AI generated design?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znh93d52m0xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1k7np7z</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Juicy fruit</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7np7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1k7n63s</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>My manicurist deserves a nobel prize I swear</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8bem2ugxzwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1k7m5xv</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Chromee</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k7m5xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1k7kfq7</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>How to get this “jelly” look</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sq66r08czwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1k7jodj</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Is this actual watercolor paint or some sort of jelly style gel polish?</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbqtwsvl5zwe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1k7ipb2</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Psychedelic vomit nail set with spinning flower</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy1dl236wywe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1k7hu9m</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>How could I get this 3D effect of the silver flowers?</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ony1eig0nywe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1k7hs17</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Ombre cloud nails ☁️</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fy5lm6bmywe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Apr 27 08:10:22 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_27.xlsx
+++ b/data/collected_data/2025_04_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1199"/>
+  <dimension ref="A1:C1375"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20816,6 +20816,2998 @@
         </is>
       </c>
     </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1k8yl2k</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Started getting my nails done recently 💅</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4sv49h2a1cxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1k8wtkz</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Can I wear this without putting polish on top?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5inoyx9dfbxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1k8w78s</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Quick press on set</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8w78s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1k8v4j4</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Paid $140 for these. Worth it?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8v4j4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1k8ve80</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>My First Gel X!</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3a27yvxyaxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1k8vcn2</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Love this set I did</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbtxvqsfyaxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1k8va55</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Some different looks I did today</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8va55</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1k8utap</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Do my nails look clean and well kept?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oehi762wsaxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1k8ufd8</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>FIRST TIMER help!</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8ufd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1k8sbwu</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>I damaged my nail bed. Should I wait until it’s completely healed to put on new press-ons?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8sbwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1k8sd50</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Inspired by the moment butter yellow is having 🧈🧈</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfyyavhh4axe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1k8tqf0</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Ethereal Witchy Nails</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqa3eymthaxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1k8u7bz</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>My partner said I have to hold something to show the birthday nails I made</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8u7bz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1k8u3gi</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Spring nails 🌷</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8u3gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1k8tvwi</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>What to ask for as someone who doesn't do nails</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8tvwi/what_to_ask_for_as_someone_who_doesnt_do_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1k8tvi2</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Fake nails</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8tvi2/fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1k8tsd6</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Yeees?💅</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mj4073eiaxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1k8tm1y</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Best 3D sculpting gel?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8tm1y/best_3d_sculpting_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1k8tk7b</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Do these look okay?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8tk7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1k8tdhf</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>regular nail polish over gel polish?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8tdhf/regular_nail_polish_over_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1k8szfi</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>First time getting nails done after almost a year and in love 💖✨️</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vo80jvxhaaxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1k8sq6x</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Wildlife enthusiast who stepped on a bee this week by accident 🥺💔 new nails were a tribute! 💛🍯🐝</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8sq6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1k8slsw</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Tried cat eye polish.. I love it! 😍</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8slsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1k8sav8</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>GelX Nails</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlmdbx5w3axe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1k8s8kd</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Tiffany blue 🩵</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96l8rfk93axe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1k8s2up</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>I absolutely love having a partner that lets me be me and express myself</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n44k5y2s1axe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1k8rx5t</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>funky flower- daisy days 💛🌼🐝</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0chhydc0axe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1k8rs0m</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Charged $50 for dip powder</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8rs0m/charged_50_for_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1k8rl32</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Game Day means Nail Day. 💅</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8rl32</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1k8r3om</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Are my nails good for a 14M? Any tips on how I can make them look better and longer?</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8r3om</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1k8r1ob</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>i did my nails for the first time in 5+ years</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8r1ob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1k8qqbi</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>What color do you recommend for my icky red undertone?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1s2ujtep9xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1k8q89u</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Advice on my Muse (Hercules) and Greek Pottery themed nails</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8q89u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1k8q63a</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Changing shape ?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8q63a/changing_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1k8obg0</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8obg0/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1k8p2fp</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Why do my nails look like this?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8p2fp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1k8p818</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>First acrylic fill ever!</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8p818</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1k8p12j</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Mystic 🩶🖤</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grrh7j9r99xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1k8os33</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Would it be weird?</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8os33/would_it_be_weird/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1k8ogu5</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>American Manicure</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8ogu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1k8oa34</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>New fill in set😍🤗</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8oa34</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1k8o8s6</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Can I put nail glue on gel polish?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8o8s6/can_i_put_nail_glue_on_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1k8o7jx</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Is my nail tech doing "apex" right?</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8o7jx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1k8ncjq</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Nail Newbie - builder gel burning?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8ncjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1k8n7wh</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Fancied a Mediterranean vibe love these!</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zi2dt0r0v8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1k8n5zk</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>You can see these from a mile away!</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8n5zk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1k8n230</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Fourth full set on my own</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qbd353frt8xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1k8mqlj</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Pastel+chrome 🤝</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8mqlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1k8mq0e</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>The worst !</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyda9ki1r8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1k8mlhs</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>These started out square</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1e8n9ctzp8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1k8m853</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>If I want to remove polish on my toes but I have professionally done poly gel nails will it mess up my nails?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqw9y820n8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1k8m7nj</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Birthday set 🎂✨✨</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5kksq4wm8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1k8m4ne</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Been obsessed with the porcelain nail art lately so I finally tried it! Added some limes for a cute cinco de mayo nail set</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7zbjxf6m8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1k8lyr3</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>I really like these ones because they suit me as well</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3dyrclvk8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1k8alef</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>What color pedicure would you do with these nails?</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8alef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1k8bhne</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Opinions</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8bhne</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1k8g2ik</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8g2ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1k8jffs</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Elven french</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8jffs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1k8l74v</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Toothpaste nails 🤣</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fs05j5poe8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1k8l5d2</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Nude nails</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6axcweae8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1k8ksto</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Pink &amp; Purple ombre w/ rainbow cat eye and glitter w/ flash</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8ksto</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1k8kseq</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Summer vibes or beach vibes? Loving this pink and glittery 3D set!</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znjl6uxdb8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1k8kqn5</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Thin nails after tips</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8kqn5/thin_nails_after_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1k8kna0</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>I love these press ons ❤️</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afbbd3aaa8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1k8keiv</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Thoughts on 'Jelly' nails?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrhoxhef88xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1k8k4ia</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Nail Shape?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8k4ia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1k8k3k5</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Last class, extension and complicated nail before and after</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8k3k5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1k8jvgq</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>got new manicure</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8jvgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1k8jnbb</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>New nails 💜🩷🩵💙</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8jnbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1k8jbyh</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Throwback to this weird salon I went to years ago</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfg54oyyz7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1k8j7ah</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Show me your nails</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9arqsezy7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1k8ir0w</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Fluid Nail Art 🎨</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8ir0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1k8ifr7</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>My sunflowers!</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ex92ku2t7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1k8goee</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>any recs on picking nails?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8goee</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1k8i8z8</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>3d fruit nails</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8i8z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1k8i861</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Color of the week!</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4smwdgmgr7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1k88i7d</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>My nails in the last 4 months. Which one do you prefer? 🌷</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k88i7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1k8csr2</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>General questions?</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8csr2/general_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1k8i1m7</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Got treated to new nails at my favorite salon today for my birthday 🥰🎉</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8i1m7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1k8fs0b</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>I love these nails but I have a question 😩</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8fs0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1k8csom</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Polygel not fully cured?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8powjrowj6xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1k8hpvj</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>First time!!!</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/appzxzijn7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1k8hpkh</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Nothing fancy! Just really like the color! 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fchop2ihn7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1k8hcw6</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Builder Gel for XXXS nail picker nails?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8hcw6/builder_gel_for_xxxs_nail_picker_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1k8guib</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Spent 3 hours on a Friday night having fun with new nail polish</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gygyeh8ug7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1k8ge73</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Testing my green nail polishes.💚</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5d3j7nzcd7xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1k8gfx4</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>First casualty of my nail growth journey :’(</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8gfx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1k8gfu9</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Infill question</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2aqpj2pd7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1k8gc6g</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Why did my professionally done cat eye nails come out like this?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkebrsoyc7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1k8g6ez</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>The satisfaction of a Fill</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8g6ez</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1k8g0yk</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>didn’t love this set initially but they started to grow on me 🥹</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jdj8bbka7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1k8fm4c</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Love my new set 😍</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8fm4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1k8fe5e</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>🍑 new set 🌸</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xozpm1ij57xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1k8f2t2</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Cada día aprendemos algo nuevo</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2clzwwz27xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1k8eby2</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Fresh set I did myself</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q42w0lj0x6xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1k8dhey</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Salon painted nails vs at home painted nails</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8dhey/salon_painted_nails_vs_at_home_painted_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1k8dd28</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Flowers are my favourite.</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6w3hva0uo6xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1k8d8zy</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>More (very) long nails!</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojprfu5xn6xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1k8cmg3</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Builder gel cracked nails - Is my new nail artist clueless?</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k8cmg3/builder_gel_cracked_nails_is_my_new_nail_artist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1k8cbdk</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Highlights of my best nails 💕</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8cbdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1k8yt3l</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Is Mooncat worth it?</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8yt3l/is_mooncat_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1k8yful</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>ATLA nail art set</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1uurzxhezbxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1k8y3af</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>What’s the history of specialty finishes and indie brands?</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8y3af/whats_the_history_of_specialty_finishes_and_indie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1k8xa3u</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Took me 2 days and a lot of redos but I finally did some nail art 👁🐍👁</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8xa3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1k8x9p6</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>What happened with the velvet?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s8qojjbskbxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1k8w205</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Does cat eye just not work on anyone else?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8w205/does_cat_eye_just_not_work_on_anyone_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1k8v21r</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Imperfect mani but SHINY</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8v21r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1k8uyhi</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Sassy sauce snake charmer</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/21l69racuaxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1k8u4ru</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Spring nails 🌷</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8u4ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1k8tm67</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Always a sucker for a blue and gold mani</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nz2j4c4ngaxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1k8t9if</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Alright…I shook them</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DI7qPD0MVuY/?igsh=MXZ2b3lyMGdpY2hjeQ==</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1k8rt1r</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Favorite magnetics?</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8rt1r/favorite_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1k8r97f</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>We don't talk about my right hand 😂</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8r97f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1k8qo1f</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Anyone’s stamper ever done this?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vuu0ixeuo9xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1k8qhht</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Mooncat Technicolor Dreams dupes?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcgzggy6n9xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1k8q29r</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Regular nail polish color similar to this photo?</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pe4ue1yej9xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1k8ph4e</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>I need to show them off somewhere</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3q1q09m8e9xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1k8pgce</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>kbshimmer get off my tail</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8pgce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1k8pbnn</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>I think I love shimmers ✨</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8pbnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1k8p8ru</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>this might be THE pink 💖</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8p8ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1k8p29d</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Can I still share my Easter mani with you?</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8p29d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1k8ore3</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>The Glow!!!</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8ore3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1k8nsmp</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Went out of my comfort zone!</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8nsmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1k8nk9t</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>top coat sadness</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8nk9t/top_coat_sadness/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1k8n7q0</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Nails I did for my son - magnet effects never this crisp on my own 😭</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cm8r7xyu8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1k8moyu</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Best drugstore polishes in the US?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8moyu/best_drugstore_polishes_in_the_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1k8lw7n</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>I only paid $8 for these!</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h84z1kpbk8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1k8lhpa</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>LA Colors “Super Bloom” made my jaw drop</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8lhpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1k8ld3e</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>My favorite combo</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8ld3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1k8l6w2</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>LA (neon jelly) Colors WHAAT</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8l6w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1k8l0tm</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>When the nails match the blooms</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ownxxg9d8xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1k8k59w</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>2 coats of HT - Made Me Ink</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8k59w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1k8kwps</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>zoya's finally having a sale...</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8kwps/zoyas_finally_having_a_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1k8kium</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>yes yes and wait yes !</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8kium</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1k8jpbb</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>🦋Nude butterflies🦋</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8jpbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1k8jkf9</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Judgment</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8jkf9/judgment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1k8jb93</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Playing with lighting: Pigment of my Imagination and Supernova</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3vgh4p43z7xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1k8iyfp</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Jellybean by ILNP</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xbptomh0x7xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1k8iw02</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>catfishing polish…</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8iw02/catfishing_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1k8isy5</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Matching Finch app to my nails</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcmrlqixv7xe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1k8iskl</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Questions about ultrafine glitters in DIY nail polish.</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8iskl/questions_about_ultrafine_glitters_in_diy_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1k8irfz</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Fluid Nail Art 🎨</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8irfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1k8hz4b</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Email from Cirque Colors</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykqkrlrhp7xe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1k8h9gf</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Polish similar to the pink on Static Nails’ “She’s Brilliant” press-ons?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oagqd1p1k7xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1k8h8c9</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Otherworldly👾👽</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8h8c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1k8h09f</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>{PR} Opposites Attract by Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8h09f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1k8gynz</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Pahlish brought back discontinued colors that differed from their originals, acknowledged these discrepancies in an email &amp; but still has not publicly addressed it.</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8gynz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1k8gyf2</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Need help identifying how to replicate this look</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8gyf2/need_help_identifying_how_to_replicate_this_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1k8guf0</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>All the cat's paws!</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8guf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1k8ezgf</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Ordering Clionadh in the US?</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8ezgf/ordering_clionadh_in_the_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1k8ejx7</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Gorgeous 😩😍 Fields of Lavender Velvet</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yffsn9uty6xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1k8dxq1</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Little watermelon moment between extensions</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8dxq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1k8dolb</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Nail polish brush replacement</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8dolb/nail_polish_brush_replacement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1k8dobo</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Someone was asking for Orly tea a few days ago...</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8dobo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1k8db1x</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>top coat necessary for water based (SOPHi) polish??</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8db1x/top_coat_necessary_for_water_based_sophi_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1k8d8vw</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Waiting in drive thru admiring the shift</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr46cqlwn6xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1k8czef</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Mooncat Rue morgue vs Essie Aruba Blue</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k8czef/mooncat_rue_morgue_vs_essie_aruba_blue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1k89wwa</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Mooncat - Forbidden Cove</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k89wwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1k89tyw</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Fyi: you need at least 2 layers of base coat</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kniljopqo5xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1k85rki</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Help me find the right pink polish for my grandma!</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k85rki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1k88fdq</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Purple goodness (and the annoying thing about tacky nails.)</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k88fdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1k8ydis</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>How can I improve?</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72evce0mybxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1k8w0rr</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Goofy little set</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9vvjkoy5bxe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1k8vqsr</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>How does mu Muse (Hercules) and Greek Pottery themed set Mock up look?</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8vqsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1k8v4rm</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>miffy nails!</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8v4rm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1k8u5y6</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Spring nails 🌷</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8u5y6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1k8sj5g</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>A friend requested these</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nccxi6546axe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1k8s2en</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>You're telling me a shrimp painted these nails?</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zo1otd1o1axe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1k8rpt0</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Vintage cake nails it took me forever!</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8rpt0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1k8r7g0</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Birthday set!</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwco6e2mt9xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1k8qc3q</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Dragon nails!!</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7kule9tl9xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1k8k67j</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Pink and silver simple for a wedding</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xbq95kk68xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1k8i74w</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8i74w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1k8htgz</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Taurus Freestyle ✨🐂 Swipe for inspo ➡️</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k8htgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1k8h1g1</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Created this set to pair with my ring</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rbct4f1ai7xe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1k8860q</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>🐸🤍</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6wtt1p735xe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>